<commit_message>
upload stock in excel fil with all conditions and edit supplier added in admin console, remaining days for delivery count automatically, order dispatch partially and full with invemtory deducion and filter added to order page for filtering the data,etc.
</commit_message>
<xml_diff>
--- a/media/Worksheet in SRS_v2.xlsx
+++ b/media/Worksheet in SRS_v2.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DADDA59E-5E3F-492A-8DF8-1E038230F75F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Django Projects\pms\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9A1CFD-6C8E-4A85-A8B7-D7645B63C11C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="19455" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query Report" sheetId="1" r:id="rId1"/>
@@ -618,7 +623,7 @@
   <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +631,7 @@
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" customWidth="1"/>
-    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -741,7 +746,7 @@
         <v>-51</v>
       </c>
       <c r="Q2" s="2">
-        <v>43669</v>
+        <v>44223</v>
       </c>
       <c r="R2">
         <v>-13</v>
@@ -806,7 +811,7 @@
         <v>-51</v>
       </c>
       <c r="Q3" s="2">
-        <v>43673</v>
+        <v>44219</v>
       </c>
       <c r="R3">
         <v>-13</v>
@@ -850,7 +855,7 @@
         <v>25</v>
       </c>
       <c r="Q4" s="2">
-        <v>43673</v>
+        <v>44218</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>